<commit_message>
Added background process handler.
</commit_message>
<xml_diff>
--- a/data/Drivers.xlsx
+++ b/data/Drivers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unomail-my.sharepoint.com/personal/isossa_unomaha_edu/Documents/FastRouting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_F25DC773A252ABDACC10485BC99F658C5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED2C36C3-8EC4-4140-9C41-1FF4067A360C}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC10485BC99F658C5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80AB8811-9D39-4B07-8D1C-EC893C02D04A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,10 +393,15 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Configured background process tooling.
</commit_message>
<xml_diff>
--- a/data/Drivers.xlsx
+++ b/data/Drivers.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unomail-my.sharepoint.com/personal/isossa_unomaha_edu/Documents/FastRouting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC10485BC99F658C5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80AB8811-9D39-4B07-8D1C-EC893C02D04A}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC10485BC99F658C5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04AD3654-6F98-4456-824E-638B185EAAB8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Alexander</t>
   </si>
@@ -73,6 +82,66 @@
   </si>
   <si>
     <t>Fernandez</t>
+  </si>
+  <si>
+    <t>Shaine</t>
+  </si>
+  <si>
+    <t>Alenin</t>
+  </si>
+  <si>
+    <t>Thurston</t>
+  </si>
+  <si>
+    <t>Wayon</t>
+  </si>
+  <si>
+    <t>Darnall</t>
+  </si>
+  <si>
+    <t>Frear</t>
+  </si>
+  <si>
+    <t>Ronalda</t>
+  </si>
+  <si>
+    <t>Carlyon</t>
+  </si>
+  <si>
+    <t>Blakeley</t>
+  </si>
+  <si>
+    <t>Gunby</t>
+  </si>
+  <si>
+    <t>Yorke</t>
+  </si>
+  <si>
+    <t>Hartington</t>
+  </si>
+  <si>
+    <t>Ryann</t>
+  </si>
+  <si>
+    <t>Britcher</t>
+  </si>
+  <si>
+    <t>Adamo</t>
+  </si>
+  <si>
+    <t>Paxton</t>
+  </si>
+  <si>
+    <t>Kristoffer</t>
+  </si>
+  <si>
+    <t>Pagan</t>
+  </si>
+  <si>
+    <t>Trevor</t>
+  </si>
+  <si>
+    <t>Ollin</t>
   </si>
 </sst>
 </file>
@@ -108,8 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,17 +462,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -480,6 +552,116 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>